<commit_message>
regular upgrade w.r.t. SpineOpt
</commit_message>
<xml_diff>
--- a/InputData/ModelConfig.xlsx
+++ b/InputData/ModelConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PhD project\Products\Models\OffPlatfEner\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8C3AB5-5BF7-4300-A410-B04A62B85E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74246934-6E2E-40CE-91E0-BC4DE157FF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6420" yWindow="22335" windowWidth="21600" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="report__output" sheetId="3" r:id="rId1"/>
@@ -237,9 +237,6 @@
     <t>db_mip_solver</t>
   </si>
   <si>
-    <t>Gurobi.jl</t>
-  </si>
-  <si>
     <t>units_invested_available</t>
   </si>
   <si>
@@ -253,6 +250,9 @@
   </si>
   <si>
     <t>2065-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>HiGHS.jl</t>
   </si>
 </sst>
 </file>
@@ -673,7 +673,7 @@
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -801,7 +801,7 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -809,7 +809,7 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -841,7 +841,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1085,7 +1085,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,13 +1132,13 @@
         <v>57</v>
       </c>
       <c r="D2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
         <v>71</v>
       </c>
-      <c r="E2" t="s">
-        <v>66</v>
-      </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w.r.t. spinetools upgrade
</commit_message>
<xml_diff>
--- a/InputData/ModelConfig.xlsx
+++ b/InputData/ModelConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PhD project\Products\Models\OffPlatfEner\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74246934-6E2E-40CE-91E0-BC4DE157FF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B77238-3D15-48E3-BD5E-9546B95EA1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="22335" windowWidth="21600" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="12645" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="report__output" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="model_relationships" sheetId="4" r:id="rId3"/>
     <sheet name="model_parameter" sheetId="7" r:id="rId4"/>
     <sheet name="temporal_block_parameter" sheetId="8" r:id="rId5"/>
+    <sheet name="scenarios" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,14 +38,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="114">
   <si>
     <t>output</t>
   </si>
   <si>
-    <t>bound_units_available</t>
-  </si>
-  <si>
     <t>bound_units_on</t>
   </si>
   <si>
@@ -63,9 +61,6 @@
     <t>constraint_units_available</t>
   </si>
   <si>
-    <t>constraint_units_on</t>
-  </si>
-  <si>
     <t>fixed_om_costs</t>
   </si>
   <si>
@@ -102,9 +97,6 @@
     <t>unit_investment_costs</t>
   </si>
   <si>
-    <t>units_available</t>
-  </si>
-  <si>
     <t>units_invested</t>
   </si>
   <si>
@@ -253,6 +245,141 @@
   </si>
   <si>
     <t>HiGHS.jl</t>
+  </si>
+  <si>
+    <t>BAU_Operation</t>
+  </si>
+  <si>
+    <t>BAU_OperationReserve</t>
+  </si>
+  <si>
+    <t>Repurposing_1</t>
+  </si>
+  <si>
+    <t>Repurposing_2</t>
+  </si>
+  <si>
+    <t>Repurposing_3</t>
+  </si>
+  <si>
+    <t>Repurposing_4</t>
+  </si>
+  <si>
+    <t>Repurposing_5</t>
+  </si>
+  <si>
+    <t>Repurposing_6</t>
+  </si>
+  <si>
+    <t>Repurposing_7</t>
+  </si>
+  <si>
+    <t>Repurposing_8</t>
+  </si>
+  <si>
+    <t>Repurposing_Reserve_1</t>
+  </si>
+  <si>
+    <t>Repurposing_Reserve_2</t>
+  </si>
+  <si>
+    <t>Repurposing_Reserve_3</t>
+  </si>
+  <si>
+    <t>Repurposing_Reserve_4</t>
+  </si>
+  <si>
+    <t>Repurposing_Reserve_5</t>
+  </si>
+  <si>
+    <t>Repurposing_Reserve_6</t>
+  </si>
+  <si>
+    <t>Repurposing_Reserve_7</t>
+  </si>
+  <si>
+    <t>Repurposing_Reserve_8</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>ContingencyExcl</t>
+  </si>
+  <si>
+    <t>ContingencyReserves</t>
+  </si>
+  <si>
+    <t>LimitLifetimeGenerator</t>
+  </si>
+  <si>
+    <t>TransitionAction</t>
+  </si>
+  <si>
+    <t>Decommission</t>
+  </si>
+  <si>
+    <t>CCS</t>
+  </si>
+  <si>
+    <t>ElectrifyBase</t>
+  </si>
+  <si>
+    <t>ElectrifyInvestWindFarm</t>
+  </si>
+  <si>
+    <t>ElectrifyPurchase</t>
+  </si>
+  <si>
+    <t>ElectrifyCCSWind</t>
+  </si>
+  <si>
+    <t>ElectrifyInvestWindFarmNoReserves</t>
+  </si>
+  <si>
+    <t>ElectrifyInvestWindFarmReserves</t>
+  </si>
+  <si>
+    <t>ElectrifyPurchaseNoReserves</t>
+  </si>
+  <si>
+    <t>ElectrifyPurchaseReserves</t>
+  </si>
+  <si>
+    <t>ElectrifyCCSWindNoReserves</t>
+  </si>
+  <si>
+    <t>ElectrifyCCSWindReserves</t>
+  </si>
+  <si>
+    <t>TSdevelopmentPersonnel_1</t>
+  </si>
+  <si>
+    <t>FixCarbonPrice_1</t>
+  </si>
+  <si>
+    <t>TSdevelopmentCarbonPrice_1</t>
+  </si>
+  <si>
+    <t>TSdevelopmentCarbonPrice_2</t>
+  </si>
+  <si>
+    <t>TSdevelopmentCarbonPrice_3</t>
+  </si>
+  <si>
+    <t>TSdevelopmentCarbonPrice_4</t>
+  </si>
+  <si>
+    <t>TSdevelopmentCarbonPrice_5</t>
+  </si>
+  <si>
+    <t>TSdevelopmentCarbonPrice_6</t>
+  </si>
+  <si>
+    <t>TSdevelopmentCarbonPrice_7</t>
+  </si>
+  <si>
+    <t>TSdevelopmentCarbonPrice_8</t>
   </si>
 </sst>
 </file>
@@ -592,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,7 +733,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -614,7 +741,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -622,15 +749,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -638,210 +765,186 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -867,24 +970,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -913,166 +1016,166 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C4" si="0">RIGHT(A2,LEN(A2)-7)</f>
         <v>report</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="0"/>
         <v>report</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
         <v>report</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C5" t="str">
         <f>RIGHT(A5,LEN(A5)-7)</f>
         <v>temporal_block</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6" t="str">
         <f>RIGHT(A6,LEN(A6)-7)</f>
         <v>temporal_block</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C7" t="str">
         <f>RIGHT(A7,LEN(A7)-7)</f>
         <v>stochastic_structure</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C8" t="str">
         <f>RIGHT(A8,LEN(A8)-15)</f>
         <v>temporal_block</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C9" t="str">
         <f>RIGHT(A9,LEN(A9)-15)</f>
         <v>stochastic_structure</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C10" t="str">
         <f>RIGHT(A10,LEN(A10)-26)</f>
         <v>temporal_block</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C11" t="str">
         <f>RIGHT(A11,LEN(A11)-26)</f>
         <v>stochastic_structure</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1084,7 +1187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AAE6B0-C091-4B9E-A9B7-F19A17B9A453}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -1100,45 +1203,45 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1167,64 +1270,991 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E6B7A9B-386D-4BAC-8278-435AB02F7397}">
+  <dimension ref="A1:S29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="29.7109375" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="29.7109375" customWidth="1"/>
+    <col min="12" max="17" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="31.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" t="s">
+        <v>52</v>
+      </c>
+      <c r="O3" t="s">
+        <v>52</v>
+      </c>
+      <c r="P3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>52</v>
+      </c>
+      <c r="R3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L5" t="s">
+        <v>89</v>
+      </c>
+      <c r="M5" t="s">
+        <v>89</v>
+      </c>
+      <c r="N5" t="s">
+        <v>89</v>
+      </c>
+      <c r="O5" t="s">
+        <v>89</v>
+      </c>
+      <c r="P5" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>89</v>
+      </c>
+      <c r="R5" t="s">
+        <v>89</v>
+      </c>
+      <c r="S5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" t="s">
+        <v>90</v>
+      </c>
+      <c r="J6" t="s">
+        <v>90</v>
+      </c>
+      <c r="K6" t="s">
+        <v>90</v>
+      </c>
+      <c r="L6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M6" t="s">
+        <v>90</v>
+      </c>
+      <c r="N6" t="s">
+        <v>90</v>
+      </c>
+      <c r="O6" t="s">
+        <v>90</v>
+      </c>
+      <c r="P6" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>90</v>
+      </c>
+      <c r="R6" t="s">
+        <v>90</v>
+      </c>
+      <c r="S6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J7" t="s">
+        <v>91</v>
+      </c>
+      <c r="K7" t="s">
+        <v>91</v>
+      </c>
+      <c r="L7" t="s">
+        <v>91</v>
+      </c>
+      <c r="M7" t="s">
+        <v>91</v>
+      </c>
+      <c r="N7" t="s">
+        <v>91</v>
+      </c>
+      <c r="O7" t="s">
+        <v>91</v>
+      </c>
+      <c r="P7" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>91</v>
+      </c>
+      <c r="R7" t="s">
+        <v>91</v>
+      </c>
+      <c r="S7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H8" t="s">
+        <v>92</v>
+      </c>
+      <c r="I8" t="s">
+        <v>92</v>
+      </c>
+      <c r="J8" t="s">
+        <v>92</v>
+      </c>
+      <c r="K8" t="s">
+        <v>92</v>
+      </c>
+      <c r="L8" t="s">
+        <v>92</v>
+      </c>
+      <c r="M8" t="s">
+        <v>92</v>
+      </c>
+      <c r="N8" t="s">
+        <v>92</v>
+      </c>
+      <c r="O8" t="s">
+        <v>92</v>
+      </c>
+      <c r="P8" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>92</v>
+      </c>
+      <c r="R8" t="s">
+        <v>92</v>
+      </c>
+      <c r="S8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" t="s">
+        <v>93</v>
+      </c>
+      <c r="J9" t="s">
+        <v>93</v>
+      </c>
+      <c r="K9" t="s">
+        <v>93</v>
+      </c>
+      <c r="L9" t="s">
+        <v>93</v>
+      </c>
+      <c r="M9" t="s">
+        <v>93</v>
+      </c>
+      <c r="N9" t="s">
+        <v>93</v>
+      </c>
+      <c r="O9" t="s">
+        <v>93</v>
+      </c>
+      <c r="P9" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>93</v>
+      </c>
+      <c r="R9" t="s">
+        <v>93</v>
+      </c>
+      <c r="S9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G10" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" t="s">
+        <v>94</v>
+      </c>
+      <c r="J10" t="s">
+        <v>94</v>
+      </c>
+      <c r="K10" t="s">
+        <v>94</v>
+      </c>
+      <c r="L10" t="s">
+        <v>94</v>
+      </c>
+      <c r="M10" t="s">
+        <v>94</v>
+      </c>
+      <c r="N10" t="s">
+        <v>94</v>
+      </c>
+      <c r="O10" t="s">
+        <v>94</v>
+      </c>
+      <c r="P10" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>94</v>
+      </c>
+      <c r="R10" t="s">
+        <v>94</v>
+      </c>
+      <c r="S10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" t="s">
+        <v>95</v>
+      </c>
+      <c r="I11" t="s">
+        <v>95</v>
+      </c>
+      <c r="J11" t="s">
+        <v>95</v>
+      </c>
+      <c r="K11" t="s">
+        <v>95</v>
+      </c>
+      <c r="L11" t="s">
+        <v>95</v>
+      </c>
+      <c r="M11" t="s">
+        <v>95</v>
+      </c>
+      <c r="N11" t="s">
+        <v>95</v>
+      </c>
+      <c r="O11" t="s">
+        <v>95</v>
+      </c>
+      <c r="P11" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>95</v>
+      </c>
+      <c r="R11" t="s">
+        <v>95</v>
+      </c>
+      <c r="S11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" t="s">
+        <v>96</v>
+      </c>
+      <c r="H12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I12" t="s">
+        <v>96</v>
+      </c>
+      <c r="J12" t="s">
+        <v>96</v>
+      </c>
+      <c r="K12" t="s">
+        <v>96</v>
+      </c>
+      <c r="L12" t="s">
+        <v>96</v>
+      </c>
+      <c r="M12" t="s">
+        <v>96</v>
+      </c>
+      <c r="N12" t="s">
+        <v>96</v>
+      </c>
+      <c r="O12" t="s">
+        <v>96</v>
+      </c>
+      <c r="P12" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>96</v>
+      </c>
+      <c r="R12" t="s">
+        <v>96</v>
+      </c>
+      <c r="S12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" t="s">
+        <v>97</v>
+      </c>
+      <c r="H13" t="s">
+        <v>97</v>
+      </c>
+      <c r="I13" t="s">
+        <v>97</v>
+      </c>
+      <c r="J13" t="s">
+        <v>97</v>
+      </c>
+      <c r="K13" t="s">
+        <v>97</v>
+      </c>
+      <c r="L13" t="s">
+        <v>97</v>
+      </c>
+      <c r="M13" t="s">
+        <v>97</v>
+      </c>
+      <c r="N13" t="s">
+        <v>97</v>
+      </c>
+      <c r="O13" t="s">
+        <v>97</v>
+      </c>
+      <c r="P13" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>97</v>
+      </c>
+      <c r="R13" t="s">
+        <v>97</v>
+      </c>
+      <c r="S13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" t="s">
+        <v>98</v>
+      </c>
+      <c r="H14" t="s">
+        <v>98</v>
+      </c>
+      <c r="I14" t="s">
+        <v>98</v>
+      </c>
+      <c r="J14" t="s">
+        <v>98</v>
+      </c>
+      <c r="K14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>99</v>
+      </c>
+      <c r="L15" t="s">
+        <v>99</v>
+      </c>
+      <c r="M15" t="s">
+        <v>99</v>
+      </c>
+      <c r="N15" t="s">
+        <v>99</v>
+      </c>
+      <c r="O15" t="s">
+        <v>99</v>
+      </c>
+      <c r="P15" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>99</v>
+      </c>
+      <c r="R15" t="s">
+        <v>99</v>
+      </c>
+      <c r="S15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G16" t="s">
+        <v>100</v>
+      </c>
+      <c r="H16" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16" t="s">
+        <v>100</v>
+      </c>
+      <c r="J16" t="s">
+        <v>100</v>
+      </c>
+      <c r="K16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>101</v>
+      </c>
+      <c r="L17" t="s">
+        <v>101</v>
+      </c>
+      <c r="M17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N17" t="s">
+        <v>101</v>
+      </c>
+      <c r="O17" t="s">
+        <v>101</v>
+      </c>
+      <c r="P17" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>101</v>
+      </c>
+      <c r="R17" t="s">
+        <v>101</v>
+      </c>
+      <c r="S17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" t="s">
+        <v>102</v>
+      </c>
+      <c r="G18" t="s">
+        <v>102</v>
+      </c>
+      <c r="H18" t="s">
+        <v>102</v>
+      </c>
+      <c r="I18" t="s">
+        <v>102</v>
+      </c>
+      <c r="J18" t="s">
+        <v>102</v>
+      </c>
+      <c r="K18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>103</v>
+      </c>
+      <c r="L19" t="s">
+        <v>103</v>
+      </c>
+      <c r="M19" t="s">
+        <v>103</v>
+      </c>
+      <c r="N19" t="s">
+        <v>103</v>
+      </c>
+      <c r="O19" t="s">
+        <v>103</v>
+      </c>
+      <c r="P19" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>103</v>
+      </c>
+      <c r="R19" t="s">
+        <v>103</v>
+      </c>
+      <c r="S19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" t="s">
+        <v>106</v>
+      </c>
+      <c r="L22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" t="s">
+        <v>107</v>
+      </c>
+      <c r="M23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24" t="s">
+        <v>108</v>
+      </c>
+      <c r="N24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>109</v>
+      </c>
+      <c r="G25" t="str">
+        <f>A25</f>
+        <v>TSdevelopmentCarbonPrice_4</v>
+      </c>
+      <c r="O25" t="str">
+        <f>A25</f>
+        <v>TSdevelopmentCarbonPrice_4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>110</v>
+      </c>
+      <c r="H26" t="str">
+        <f>A26</f>
+        <v>TSdevelopmentCarbonPrice_5</v>
+      </c>
+      <c r="P26" t="str">
+        <f>A26</f>
+        <v>TSdevelopmentCarbonPrice_5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>111</v>
+      </c>
+      <c r="I27" t="str">
+        <f>A27</f>
+        <v>TSdevelopmentCarbonPrice_6</v>
+      </c>
+      <c r="Q27" t="str">
+        <f>A27</f>
+        <v>TSdevelopmentCarbonPrice_6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>112</v>
+      </c>
+      <c r="J28" t="str">
+        <f>A28</f>
+        <v>TSdevelopmentCarbonPrice_7</v>
+      </c>
+      <c r="R28" t="str">
+        <f>A28</f>
+        <v>TSdevelopmentCarbonPrice_7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>113</v>
+      </c>
+      <c r="K29" t="str">
+        <f>A29</f>
+        <v>TSdevelopmentCarbonPrice_8</v>
+      </c>
+      <c r="S29" t="str">
+        <f>A29</f>
+        <v>TSdevelopmentCarbonPrice_8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>